<commit_message>
upload orgincode detecting result
</commit_message>
<xml_diff>
--- a/res_img/resnet50-3way-10k-size(768)-medium/动态.xlsx
+++ b/res_img/resnet50-3way-10k-size(768)-medium/动态.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Remote_GDJC\res_img\resnet50-3way-10k-size(768)-medium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2633A8-4924-4F90-A892-1B6F163FB19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1339C3-8E2E-484F-B6D3-2BD5223AE055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1531,16 +1531,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2722</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>97971</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>655865</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>394607</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>146956</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>351065</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1831,15 +1831,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>0.106</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>0.14199999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>0.14899999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2076,8 +2076,14 @@
       <c r="E14">
         <v>0.22</v>
       </c>
+      <c r="F14">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="G14">
+        <v>0.57599999999999996</v>
+      </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2093,8 +2099,14 @@
       <c r="E15">
         <v>0.184</v>
       </c>
+      <c r="F15">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.62</v>
+      </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2109,6 +2121,38 @@
       </c>
       <c r="E16">
         <v>0.124</v>
+      </c>
+      <c r="F16">
+        <v>0.748</v>
+      </c>
+      <c r="G16">
+        <v>0.59799999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <f>SUM(B14:B16)/3</f>
+        <v>0.56733333333333336</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:F18" si="0">SUM(C14:C16)/3</f>
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0.6336666666666666</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.17600000000000002</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.73999999999999988</v>
+      </c>
+      <c r="G18">
+        <f>SUM(G14:G16)/3</f>
+        <v>0.59799999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>